<commit_message>
Remove deficit mindset/ add 2027, add new ICS data to 2023
</commit_message>
<xml_diff>
--- a/LakeMeadStorageICS/IntentionallyCreatedSurplus-Summary.xlsx
+++ b/LakeMeadStorageICS/IntentionallyCreatedSurplus-Summary.xlsx
@@ -1,34 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20375"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverFutures\MeadPowellPlots\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadStorageICS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D529D4-00BE-47FB-9B33-28155E674629}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23FF1E6-7E50-4B4C-9D47-4C3F6BFEC3D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20520" yWindow="-2640" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="ICStoDCP" sheetId="3" r:id="rId2"/>
-    <sheet name="DCPLogs" sheetId="4" r:id="rId3"/>
-    <sheet name="By User" sheetId="2" r:id="rId4"/>
+    <sheet name="Capacities" sheetId="5" r:id="rId2"/>
+    <sheet name="ICStoDCP" sheetId="3" r:id="rId3"/>
+    <sheet name="DCPLogs" sheetId="4" r:id="rId4"/>
+    <sheet name="By User" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="65">
   <si>
     <t>Data Sources:</t>
   </si>
@@ -211,6 +223,18 @@
   </si>
   <si>
     <t>CAWCD</t>
+  </si>
+  <si>
+    <t>US+MX</t>
+  </si>
+  <si>
+    <t>Balance - Dec 2021 (AF)</t>
+  </si>
+  <si>
+    <t>Balance - Dec 2022 (AF)</t>
+  </si>
+  <si>
+    <t>Balance - Dec 2023 (AF)</t>
   </si>
 </sst>
 </file>
@@ -304,7 +328,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -314,22 +338,20 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -344,22 +366,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -647,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -659,10 +678,11 @@
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="5" width="10.54296875" customWidth="1"/>
-    <col min="6" max="6" width="10.36328125" customWidth="1"/>
-    <col min="7" max="7" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.54296875" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.81640625" customWidth="1"/>
     <col min="10" max="10" width="9.81640625" customWidth="1"/>
+    <col min="14" max="14" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -686,12 +706,12 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="H5" s="26" t="s">
+      <c r="H5" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
     </row>
     <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
@@ -706,7 +726,7 @@
       <c r="D6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="3" t="s">
         <v>52</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -727,311 +747,338 @@
       <c r="K6" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="L6" s="22" t="s">
+      <c r="L6" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="23">
-        <v>598742</v>
-      </c>
-      <c r="C7" s="23">
-        <v>1375871</v>
-      </c>
-      <c r="D7" s="23">
-        <v>865741</v>
-      </c>
-      <c r="E7" s="23">
-        <f>41000+E8</f>
-        <v>173975</v>
+      <c r="N6" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="3">
+        <v>710589</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1661832</v>
+      </c>
+      <c r="D7" s="3">
+        <v>955543</v>
+      </c>
+      <c r="E7" s="21">
+        <f>E8-34000</f>
+        <v>210975</v>
       </c>
       <c r="F7" s="2">
-        <f>SUM(B7:D7)</f>
-        <v>2840354</v>
-      </c>
-      <c r="G7" s="24">
-        <v>2020</v>
-      </c>
-      <c r="H7" s="12">
+        <f t="shared" ref="F7:F9" si="0">SUM(B7:D7)</f>
+        <v>3327964</v>
+      </c>
+      <c r="G7" s="1">
+        <v>2023</v>
+      </c>
+      <c r="H7" s="11">
         <f>F7-F8</f>
-        <v>527727</v>
-      </c>
-      <c r="I7" s="20">
-        <f t="shared" ref="I7:L8" si="0">B7-B8</f>
-        <v>125238</v>
-      </c>
-      <c r="J7" s="20">
+        <v>290083</v>
+      </c>
+      <c r="I7" s="18">
+        <f t="shared" ref="I7" si="1">B7-B8</f>
+        <v>-42834</v>
+      </c>
+      <c r="J7" s="18">
+        <f t="shared" ref="J7" si="2">C7-C8</f>
+        <v>416139</v>
+      </c>
+      <c r="K7" s="18">
+        <f t="shared" ref="K7" si="3">D7-D8</f>
+        <v>-83222</v>
+      </c>
+      <c r="L7" s="18">
+        <f t="shared" ref="L7" si="4">E7-E8</f>
+        <v>-34000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="12">
+        <v>753423</v>
+      </c>
+      <c r="C8" s="12">
+        <v>1245693</v>
+      </c>
+      <c r="D8" s="12">
+        <v>1038765</v>
+      </c>
+      <c r="E8" s="19">
+        <f>30000+E9</f>
+        <v>244975</v>
+      </c>
+      <c r="F8" s="2">
         <f t="shared" si="0"/>
-        <v>322661</v>
-      </c>
-      <c r="K7" s="20">
+        <v>3037881</v>
+      </c>
+      <c r="G8" s="20">
+        <v>2022</v>
+      </c>
+      <c r="H8" s="11">
+        <f>F8-F9</f>
+        <v>46937</v>
+      </c>
+      <c r="I8" s="18">
+        <f t="shared" ref="I8:I9" si="5">B8-B9</f>
+        <v>69222</v>
+      </c>
+      <c r="J8" s="18">
+        <f t="shared" ref="J8:J9" si="6">C8-C9</f>
+        <v>-111392</v>
+      </c>
+      <c r="K8" s="18">
+        <f t="shared" ref="K8:K9" si="7">D8-D9</f>
+        <v>89107</v>
+      </c>
+      <c r="L8" s="18">
+        <f t="shared" ref="L8:L9" si="8">E8-E9</f>
+        <v>30000</v>
+      </c>
+      <c r="N8" s="11">
+        <f t="shared" ref="N8:N9" si="9">SUM(E8:F8)</f>
+        <v>3282856</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="12">
+        <v>684201</v>
+      </c>
+      <c r="C9" s="12">
+        <v>1357085</v>
+      </c>
+      <c r="D9" s="12">
+        <v>949658</v>
+      </c>
+      <c r="E9" s="19">
+        <f>41000+E10</f>
+        <v>214975</v>
+      </c>
+      <c r="F9" s="2">
         <f t="shared" si="0"/>
-        <v>79828</v>
-      </c>
-      <c r="L7" s="20">
-        <f t="shared" si="0"/>
+        <v>2990944</v>
+      </c>
+      <c r="G9" s="20">
+        <v>2021</v>
+      </c>
+      <c r="H9" s="11">
+        <f t="shared" ref="H9" si="10">F9-F10</f>
+        <v>150590</v>
+      </c>
+      <c r="I9" s="18">
+        <f t="shared" si="5"/>
+        <v>85459</v>
+      </c>
+      <c r="J9" s="18">
+        <f t="shared" si="6"/>
+        <v>-18786</v>
+      </c>
+      <c r="K9" s="18">
+        <f t="shared" si="7"/>
+        <v>83917</v>
+      </c>
+      <c r="L9" s="18">
+        <f t="shared" si="8"/>
         <v>41000</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G8,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>473504</v>
-      </c>
-      <c r="C8" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G8,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>1053210</v>
-      </c>
-      <c r="D8" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G8,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>785913</v>
-      </c>
-      <c r="E8" s="2">
-        <v>132975</v>
-      </c>
-      <c r="F8" s="2">
-        <f>SUM(B8:D8)</f>
-        <v>2312627</v>
-      </c>
-      <c r="G8" s="14">
-        <v>2019</v>
-      </c>
-      <c r="H8" s="12">
-        <f>F8-F9</f>
-        <v>570695</v>
-      </c>
-      <c r="I8" s="20">
-        <f t="shared" si="0"/>
-        <v>130452</v>
-      </c>
-      <c r="J8" s="20">
-        <f t="shared" si="0"/>
-        <v>354778</v>
-      </c>
-      <c r="K8" s="20">
-        <f t="shared" si="0"/>
-        <v>85465</v>
-      </c>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20">
-        <f>H8-H7</f>
-        <v>42968</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G9,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>343052</v>
-      </c>
-      <c r="C9" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G9,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>698432</v>
-      </c>
-      <c r="D9" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G9,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>700448</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2">
-        <f>SUM(B9:D9)</f>
-        <v>1741932</v>
-      </c>
-      <c r="G9" s="10">
-        <v>2018</v>
-      </c>
-      <c r="H9" s="12">
-        <f>F9-F10</f>
-        <v>480441</v>
-      </c>
-      <c r="I9" s="20">
-        <f t="shared" ref="I9:I16" si="1">B9-B10</f>
-        <v>216252</v>
-      </c>
-      <c r="J9" s="20">
-        <f t="shared" ref="J9:J16" si="2">C9-C10</f>
-        <v>146054</v>
-      </c>
-      <c r="K9" s="20">
-        <f t="shared" ref="K9:K16" si="3">D9-D10</f>
-        <v>118135</v>
+      <c r="N9" s="11">
+        <f t="shared" si="9"/>
+        <v>3205919</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G10,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>126800</v>
-      </c>
-      <c r="C10" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G10,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>552378</v>
-      </c>
-      <c r="D10" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G10,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>582313</v>
-      </c>
-      <c r="E10" s="2"/>
+        <v>51</v>
+      </c>
+      <c r="B10" s="19">
+        <v>598742</v>
+      </c>
+      <c r="C10" s="19">
+        <v>1375871</v>
+      </c>
+      <c r="D10" s="19">
+        <v>865741</v>
+      </c>
+      <c r="E10" s="19">
+        <f>41000+E11</f>
+        <v>173975</v>
+      </c>
       <c r="F10" s="2">
         <f>SUM(B10:D10)</f>
-        <v>1261491</v>
-      </c>
-      <c r="G10" s="11">
-        <v>2017</v>
-      </c>
-      <c r="H10" s="12">
-        <f t="shared" ref="H10:H16" si="4">F10-F11</f>
-        <v>511813</v>
-      </c>
-      <c r="I10" s="20">
-        <f t="shared" si="1"/>
-        <v>23750</v>
-      </c>
-      <c r="J10" s="20">
-        <f t="shared" si="2"/>
-        <v>437312</v>
-      </c>
-      <c r="K10" s="20">
-        <f t="shared" si="3"/>
-        <v>50751</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+        <v>2840354</v>
+      </c>
+      <c r="G10" s="20">
+        <v>2020</v>
+      </c>
+      <c r="H10" s="11">
+        <f>F10-F11</f>
+        <v>527727</v>
+      </c>
+      <c r="I10" s="18">
+        <f t="shared" ref="I10:L11" si="11">B10-B11</f>
+        <v>125238</v>
+      </c>
+      <c r="J10" s="18">
+        <f t="shared" si="11"/>
+        <v>322661</v>
+      </c>
+      <c r="K10" s="18">
+        <f t="shared" si="11"/>
+        <v>79828</v>
+      </c>
+      <c r="L10" s="18">
+        <f t="shared" si="11"/>
+        <v>41000</v>
+      </c>
+      <c r="N10" s="11">
+        <f>SUM(E10:F10)</f>
+        <v>3014329</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B11" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G11,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>103050</v>
+        <v>473504</v>
       </c>
       <c r="C11" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G11,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>115066</v>
+        <v>1053210</v>
       </c>
       <c r="D11" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G11,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>531562</v>
-      </c>
-      <c r="E11" s="2"/>
+        <v>785913</v>
+      </c>
+      <c r="E11" s="2">
+        <v>132975</v>
+      </c>
       <c r="F11" s="2">
-        <f t="shared" ref="F11:F17" si="5">SUM(B11:D11)</f>
-        <v>749678</v>
-      </c>
-      <c r="G11" s="11">
-        <v>2016</v>
-      </c>
-      <c r="H11" s="12">
-        <f t="shared" si="4"/>
-        <v>37814</v>
-      </c>
-      <c r="I11" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="20">
-        <f t="shared" si="2"/>
-        <v>17275</v>
-      </c>
-      <c r="K11" s="20">
-        <f t="shared" si="3"/>
-        <v>20539</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+        <f>SUM(B11:D11)</f>
+        <v>2312627</v>
+      </c>
+      <c r="G11" s="12">
+        <v>2019</v>
+      </c>
+      <c r="H11" s="11">
+        <f>F11-F12</f>
+        <v>570695</v>
+      </c>
+      <c r="I11" s="18">
+        <f t="shared" si="11"/>
+        <v>130452</v>
+      </c>
+      <c r="J11" s="18">
+        <f t="shared" si="11"/>
+        <v>354778</v>
+      </c>
+      <c r="K11" s="18">
+        <f t="shared" si="11"/>
+        <v>85465</v>
+      </c>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18">
+        <f>H11-H10</f>
+        <v>42968</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B12" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G12,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>103050</v>
+        <v>343052</v>
       </c>
       <c r="C12" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G12,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>97791</v>
+        <v>698432</v>
       </c>
       <c r="D12" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G12,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>511023</v>
+        <v>700448</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2">
-        <f t="shared" si="5"/>
-        <v>711864</v>
-      </c>
-      <c r="G12" s="11">
-        <v>2015</v>
-      </c>
-      <c r="H12" s="12">
-        <f t="shared" si="4"/>
-        <v>-125036</v>
-      </c>
-      <c r="I12" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="20">
-        <f t="shared" si="2"/>
-        <v>-71294</v>
-      </c>
-      <c r="K12" s="20">
-        <f t="shared" si="3"/>
-        <v>-53742</v>
+        <f>SUM(B12:D12)</f>
+        <v>1741932</v>
+      </c>
+      <c r="G12" s="9">
+        <v>2018</v>
+      </c>
+      <c r="H12" s="11">
+        <f>F12-F13</f>
+        <v>480441</v>
+      </c>
+      <c r="I12" s="18">
+        <f t="shared" ref="I12:I19" si="12">B12-B13</f>
+        <v>216252</v>
+      </c>
+      <c r="J12" s="18">
+        <f t="shared" ref="J12:J19" si="13">C12-C13</f>
+        <v>146054</v>
+      </c>
+      <c r="K12" s="18">
+        <f t="shared" ref="K12:K19" si="14">D12-D13</f>
+        <v>118135</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B13" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G13,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>103050</v>
+        <v>126800</v>
       </c>
       <c r="C13" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G13,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>169085</v>
+        <v>552378</v>
       </c>
       <c r="D13" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G13,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>564765</v>
+        <v>582313</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2">
-        <f t="shared" si="5"/>
-        <v>836900</v>
-      </c>
-      <c r="G13" s="11">
-        <v>2014</v>
-      </c>
-      <c r="H13" s="12">
-        <f t="shared" si="4"/>
-        <v>-281264</v>
-      </c>
-      <c r="I13" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="20">
-        <f t="shared" si="2"/>
-        <v>-304978</v>
-      </c>
-      <c r="K13" s="20">
-        <f t="shared" si="3"/>
-        <v>23714</v>
+        <f>SUM(B13:D13)</f>
+        <v>1261491</v>
+      </c>
+      <c r="G13" s="10">
+        <v>2017</v>
+      </c>
+      <c r="H13" s="11">
+        <f t="shared" ref="H13:H19" si="15">F13-F14</f>
+        <v>511813</v>
+      </c>
+      <c r="I13" s="18">
+        <f t="shared" si="12"/>
+        <v>23750</v>
+      </c>
+      <c r="J13" s="18">
+        <f t="shared" si="13"/>
+        <v>437312</v>
+      </c>
+      <c r="K13" s="18">
+        <f t="shared" si="14"/>
+        <v>50751</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G14,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
@@ -1039,40 +1086,40 @@
       </c>
       <c r="C14" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G14,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>474063</v>
+        <v>115066</v>
       </c>
       <c r="D14" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G14,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>541051</v>
+        <v>531562</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2">
-        <f t="shared" si="5"/>
-        <v>1118164</v>
-      </c>
-      <c r="G14" s="11">
-        <v>2013</v>
-      </c>
-      <c r="H14" s="12">
-        <f t="shared" si="4"/>
-        <v>-77476</v>
-      </c>
-      <c r="I14" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F14:F20" si="16">SUM(B14:D14)</f>
+        <v>749678</v>
+      </c>
+      <c r="G14" s="10">
+        <v>2016</v>
+      </c>
+      <c r="H14" s="11">
+        <f t="shared" si="15"/>
+        <v>37814</v>
+      </c>
+      <c r="I14" s="18">
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="J14" s="20">
-        <f t="shared" si="2"/>
-        <v>-105723</v>
-      </c>
-      <c r="K14" s="20">
-        <f t="shared" si="3"/>
-        <v>28247</v>
+      <c r="J14" s="18">
+        <f t="shared" si="13"/>
+        <v>17275</v>
+      </c>
+      <c r="K14" s="18">
+        <f t="shared" si="14"/>
+        <v>20539</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B15" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G15,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
@@ -1080,40 +1127,40 @@
       </c>
       <c r="C15" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G15,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>579786</v>
+        <v>97791</v>
       </c>
       <c r="D15" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G15,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>512804</v>
+        <v>511023</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2">
-        <f t="shared" si="5"/>
-        <v>1195640</v>
-      </c>
-      <c r="G15" s="11">
-        <v>2012</v>
-      </c>
-      <c r="H15" s="12">
-        <f t="shared" si="4"/>
-        <v>169240</v>
-      </c>
-      <c r="I15" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
+        <v>711864</v>
+      </c>
+      <c r="G15" s="10">
+        <v>2015</v>
+      </c>
+      <c r="H15" s="11">
+        <f t="shared" si="15"/>
+        <v>-125036</v>
+      </c>
+      <c r="I15" s="18">
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="J15" s="20">
-        <f t="shared" si="2"/>
-        <v>139108</v>
-      </c>
-      <c r="K15" s="20">
-        <f t="shared" si="3"/>
-        <v>30132</v>
+      <c r="J15" s="18">
+        <f t="shared" si="13"/>
+        <v>-71294</v>
+      </c>
+      <c r="K15" s="18">
+        <f t="shared" si="14"/>
+        <v>-53742</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B16" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G16,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
@@ -1121,284 +1168,188 @@
       </c>
       <c r="C16" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G16,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>440678</v>
+        <v>169085</v>
       </c>
       <c r="D16" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G16,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>482672</v>
+        <v>564765</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2">
-        <f t="shared" si="5"/>
-        <v>1026400</v>
-      </c>
-      <c r="G16" s="11">
-        <v>2011</v>
-      </c>
-      <c r="H16" s="12">
-        <f t="shared" si="4"/>
-        <v>211059</v>
-      </c>
-      <c r="I16" s="20">
-        <f t="shared" si="1"/>
-        <v>956</v>
-      </c>
-      <c r="J16" s="20">
-        <f t="shared" si="2"/>
-        <v>178688</v>
-      </c>
-      <c r="K16" s="20">
-        <f t="shared" si="3"/>
-        <v>31415</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+        <f t="shared" si="16"/>
+        <v>836900</v>
+      </c>
+      <c r="G16" s="10">
+        <v>2014</v>
+      </c>
+      <c r="H16" s="11">
+        <f t="shared" si="15"/>
+        <v>-281264</v>
+      </c>
+      <c r="I16" s="18">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="18">
+        <f t="shared" si="13"/>
+        <v>-304978</v>
+      </c>
+      <c r="K16" s="18">
+        <f t="shared" si="14"/>
+        <v>23714</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B17" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G17,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>102094</v>
+        <v>103050</v>
       </c>
       <c r="C17" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G17,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>261990</v>
+        <v>474063</v>
       </c>
       <c r="D17" s="2">
         <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G17,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>451257</v>
+        <v>541051</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2">
-        <f t="shared" si="5"/>
-        <v>815341</v>
-      </c>
-      <c r="G17" s="11">
-        <v>2010</v>
-      </c>
-      <c r="H17" s="12"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+        <f t="shared" si="16"/>
+        <v>1118164</v>
+      </c>
+      <c r="G17" s="10">
+        <v>2013</v>
+      </c>
+      <c r="H17" s="11">
+        <f t="shared" si="15"/>
+        <v>-77476</v>
+      </c>
+      <c r="I17" s="18">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="18">
+        <f t="shared" si="13"/>
+        <v>-105723</v>
+      </c>
+      <c r="K17" s="18">
+        <f t="shared" si="14"/>
+        <v>28247</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B18" s="2">
-        <v>100000</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G18,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
+        <v>103050</v>
       </c>
       <c r="C18" s="2">
-        <v>400000</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G18,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
+        <v>579786</v>
       </c>
       <c r="D18" s="2">
-        <v>125000</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G18,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
+        <v>512804</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2">
-        <f t="shared" ref="F18:F20" si="6">SUM(B18:D18)</f>
-        <v>625000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+        <f t="shared" si="16"/>
+        <v>1195640</v>
+      </c>
+      <c r="G18" s="10">
+        <v>2012</v>
+      </c>
+      <c r="H18" s="11">
+        <f t="shared" si="15"/>
+        <v>169240</v>
+      </c>
+      <c r="I18" s="18">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="18">
+        <f t="shared" si="13"/>
+        <v>139108</v>
+      </c>
+      <c r="K18" s="18">
+        <f t="shared" si="14"/>
+        <v>30132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="B19" s="2">
-        <v>300000</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G19,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
+        <v>103050</v>
       </c>
       <c r="C19" s="2">
-        <v>1500000</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G19,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
+        <v>440678</v>
       </c>
       <c r="D19" s="2">
-        <v>300000</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G19,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
+        <v>482672</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2">
-        <f t="shared" si="6"/>
-        <v>2100000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+        <f t="shared" si="16"/>
+        <v>1026400</v>
+      </c>
+      <c r="G19" s="10">
+        <v>2011</v>
+      </c>
+      <c r="H19" s="11">
+        <f t="shared" si="15"/>
+        <v>211059</v>
+      </c>
+      <c r="I19" s="18">
+        <f t="shared" si="12"/>
+        <v>956</v>
+      </c>
+      <c r="J19" s="18">
+        <f t="shared" si="13"/>
+        <v>178688</v>
+      </c>
+      <c r="K19" s="18">
+        <f t="shared" si="14"/>
+        <v>31415</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B20" s="2">
-        <v>300000</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G20,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
+        <v>102094</v>
       </c>
       <c r="C20" s="2">
-        <v>400000</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G20,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
+        <v>261990</v>
       </c>
       <c r="D20" s="2">
-        <v>300000</v>
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G20,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
+        <v>451257</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2">
-        <f t="shared" si="6"/>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="9" t="str">
-        <f>B6</f>
-        <v>Arizona</v>
-      </c>
-      <c r="C23" s="9" t="str">
-        <f t="shared" ref="C23:F23" si="7">C6</f>
-        <v>California</v>
-      </c>
-      <c r="D23" s="9" t="str">
-        <f t="shared" si="7"/>
-        <v>Nevada</v>
-      </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9" t="str">
-        <f t="shared" si="7"/>
-        <v>Total</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24" s="7">
-        <v>100000</v>
-      </c>
-      <c r="C24" s="7">
-        <v>400000</v>
-      </c>
-      <c r="D24" s="7">
-        <v>125000</v>
-      </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7">
-        <f t="shared" ref="F24:F26" si="8">SUM(B24:D24)</f>
-        <v>625000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="7">
-        <v>500000</v>
-      </c>
-      <c r="C25" s="7">
-        <v>1700000</v>
-      </c>
-      <c r="D25" s="7">
-        <v>500000</v>
-      </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7">
-        <f t="shared" si="8"/>
-        <v>2700000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="7">
-        <f>B20</f>
-        <v>300000</v>
-      </c>
-      <c r="C26" s="7">
-        <f t="shared" ref="C26:D26" si="9">C20</f>
-        <v>400000</v>
-      </c>
-      <c r="D26" s="7">
-        <f t="shared" si="9"/>
-        <v>300000</v>
-      </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7">
-        <f t="shared" si="8"/>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>11</v>
-      </c>
-      <c r="B31" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="C31" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="D31" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="E31" s="4"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>17</v>
-      </c>
-      <c r="B32" s="4">
-        <v>0.03</v>
-      </c>
-      <c r="C32" s="4">
-        <v>0.03</v>
-      </c>
-      <c r="D32" s="4">
-        <v>0.03</v>
-      </c>
-      <c r="E32" s="4"/>
+        <f t="shared" si="16"/>
+        <v>815341</v>
+      </c>
+      <c r="G20" s="10">
+        <v>2010</v>
+      </c>
+      <c r="H20" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A27:F27"/>
+  <mergeCells count="1">
     <mergeCell ref="H5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1406,26 +1357,290 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F9C09D6-2BEE-4EAC-9C47-48919B4DAC3E}">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.7265625" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="6" max="6" width="10.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2">
+        <v>100000</v>
+      </c>
+      <c r="C2" s="2">
+        <v>400000</v>
+      </c>
+      <c r="D2" s="2">
+        <v>125000</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2">
+        <f t="shared" ref="F2:F4" si="0">SUM(B2:D2)</f>
+        <v>625000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2">
+        <v>300000</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1500000</v>
+      </c>
+      <c r="D3" s="2">
+        <v>300000</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2">
+        <f t="shared" si="0"/>
+        <v>2100000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2">
+        <v>300000</v>
+      </c>
+      <c r="C4" s="2">
+        <v>400000</v>
+      </c>
+      <c r="D4" s="2">
+        <v>300000</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2">
+        <f t="shared" si="0"/>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="8" t="str">
+        <f>B1</f>
+        <v>Arizona</v>
+      </c>
+      <c r="C7" s="8" t="str">
+        <f t="shared" ref="C7:F7" si="1">C1</f>
+        <v>California</v>
+      </c>
+      <c r="D7" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Nevada</v>
+      </c>
+      <c r="E7" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Mexico</v>
+      </c>
+      <c r="F7" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Total</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="6">
+        <v>100000</v>
+      </c>
+      <c r="C8" s="6">
+        <v>400000</v>
+      </c>
+      <c r="D8" s="6">
+        <v>125000</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6">
+        <f t="shared" ref="F8:F10" si="2">SUM(B8:D8)</f>
+        <v>625000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="6">
+        <v>500000</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1700000</v>
+      </c>
+      <c r="D9" s="6">
+        <v>500000</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6">
+        <f t="shared" si="2"/>
+        <v>2700000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="6">
+        <f>B4</f>
+        <v>300000</v>
+      </c>
+      <c r="C10" s="6">
+        <f t="shared" ref="C10:D10" si="3">C4</f>
+        <v>400000</v>
+      </c>
+      <c r="D10" s="6">
+        <f t="shared" si="3"/>
+        <v>300000</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6">
+        <f t="shared" si="2"/>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="E16" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A11:F11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F1C2B7-EA8A-46B6-A876-EE2A69C03180}">
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="9.7265625" customWidth="1"/>
-    <col min="3" max="3" width="10.08984375" customWidth="1"/>
-    <col min="4" max="4" width="9.6328125" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" customWidth="1"/>
+    <col min="4" max="4" width="9.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
       <c r="H1" t="s">
         <v>48</v>
       </c>
@@ -1434,443 +1649,443 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="M2" s="13" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="16">
+      <c r="A3" s="14">
         <v>1218.5</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="16">
+      <c r="A4" s="14">
         <v>1190</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" s="16">
+      <c r="A5" s="14">
         <v>1150</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="7">
+      <c r="A6" s="6">
         <v>1091</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="7">
+      <c r="A7" s="6">
         <v>1090</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>192000</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6">
         <v>8000</v>
       </c>
-      <c r="E7" s="17">
-        <f>Sheet1!B$7/B7</f>
+      <c r="E7" s="15">
+        <f>Sheet1!B$10/B7</f>
         <v>3.1184479166666668</v>
       </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17">
-        <f>Sheet1!D$7/D7</f>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15">
+        <f>Sheet1!D$10/D7</f>
         <v>108.217625</v>
       </c>
-      <c r="H7" s="19">
-        <f>Sheet1!B$26/ICStoDCP!B7</f>
-        <v>1.5625</v>
-      </c>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19">
-        <f>Sheet1!D$26/ICStoDCP!D7</f>
-        <v>37.5</v>
-      </c>
-      <c r="K7" s="18">
-        <f>Sheet1!B$24/ICStoDCP!B7</f>
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18">
-        <f>Sheet1!D$24/ICStoDCP!D7</f>
-        <v>15.625</v>
+      <c r="H7" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B7</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D7</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K7" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B7</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D7</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" s="7">
+      <c r="A8" s="6">
         <v>1075</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>512000</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7">
+      <c r="C8" s="6"/>
+      <c r="D8" s="6">
         <v>21000</v>
       </c>
-      <c r="E8" s="17">
-        <f>Sheet1!B$7/B8</f>
+      <c r="E8" s="15">
+        <f>Sheet1!B$10/B8</f>
         <v>1.1694179687499999</v>
       </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17">
-        <f>Sheet1!D$7/D8</f>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15">
+        <f>Sheet1!D$10/D8</f>
         <v>41.225761904761903</v>
       </c>
-      <c r="H8" s="19">
-        <f>Sheet1!B$26/ICStoDCP!B8</f>
-        <v>0.5859375</v>
-      </c>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19">
-        <f>Sheet1!D$26/ICStoDCP!D8</f>
-        <v>14.285714285714286</v>
-      </c>
-      <c r="K8" s="18">
-        <f>Sheet1!B$24/ICStoDCP!B8</f>
-        <v>0.1953125</v>
-      </c>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18">
-        <f>Sheet1!D$24/ICStoDCP!D8</f>
-        <v>5.9523809523809526</v>
+      <c r="H8" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B8</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D8</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K8" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B8</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D8</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="7">
+      <c r="A9" s="6">
         <v>1050</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>592000</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7">
+      <c r="C9" s="6"/>
+      <c r="D9" s="6">
         <v>25000</v>
       </c>
-      <c r="E9" s="17">
-        <f>Sheet1!B$7/B9</f>
+      <c r="E9" s="15">
+        <f>Sheet1!B$10/B9</f>
         <v>1.0113885135135134</v>
       </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17">
-        <f>Sheet1!D$7/D9</f>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15">
+        <f>Sheet1!D$10/D9</f>
         <v>34.629640000000002</v>
       </c>
-      <c r="H9" s="19">
-        <f>Sheet1!B$26/ICStoDCP!B9</f>
-        <v>0.5067567567567568</v>
-      </c>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19">
-        <f>Sheet1!D$26/ICStoDCP!D9</f>
-        <v>12</v>
-      </c>
-      <c r="K9" s="18">
-        <f>Sheet1!B$24/ICStoDCP!B9</f>
-        <v>0.16891891891891891</v>
-      </c>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18">
-        <f>Sheet1!D$24/ICStoDCP!D9</f>
-        <v>5</v>
+      <c r="H9" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B9</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D9</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K9" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B9</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D9</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" s="7">
+      <c r="A10" s="6">
         <v>1045</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>640000</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>200000</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="6">
         <v>27000</v>
       </c>
-      <c r="E10" s="17">
-        <f>Sheet1!B$7/B10</f>
+      <c r="E10" s="15">
+        <f>Sheet1!B$10/B10</f>
         <v>0.93553437500000003</v>
       </c>
-      <c r="F10" s="17">
-        <f>Sheet1!C$7/C10</f>
+      <c r="F10" s="15">
+        <f>Sheet1!C$10/C10</f>
         <v>6.8793550000000003</v>
       </c>
-      <c r="G10" s="17">
-        <f>Sheet1!D$7/D10</f>
+      <c r="G10" s="15">
+        <f>Sheet1!D$10/D10</f>
         <v>32.064481481481479</v>
       </c>
-      <c r="H10" s="19">
-        <f>Sheet1!B$26/ICStoDCP!B10</f>
-        <v>0.46875</v>
-      </c>
-      <c r="I10" s="19">
-        <f>Sheet1!C$26/ICStoDCP!C10</f>
-        <v>2</v>
-      </c>
-      <c r="J10" s="19">
-        <f>Sheet1!D$26/ICStoDCP!D10</f>
-        <v>11.111111111111111</v>
-      </c>
-      <c r="K10" s="18">
-        <f>Sheet1!B$24/ICStoDCP!B10</f>
-        <v>0.15625</v>
-      </c>
-      <c r="L10" s="18">
-        <f>Sheet1!C$24/ICStoDCP!C10</f>
-        <v>2</v>
-      </c>
-      <c r="M10" s="18">
-        <f>Sheet1!D$24/ICStoDCP!D10</f>
-        <v>4.6296296296296298</v>
+      <c r="H10" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B10</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I10" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!C10</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J10" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D10</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K10" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B10</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L10" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!C10</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M10" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D10</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" s="7">
+      <c r="A11" s="6">
         <v>1040</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <v>640000</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>250000</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="6">
         <v>27000</v>
       </c>
-      <c r="E11" s="17">
-        <f>Sheet1!B$7/B11</f>
+      <c r="E11" s="15">
+        <f>Sheet1!B$10/B11</f>
         <v>0.93553437500000003</v>
       </c>
-      <c r="F11" s="17">
-        <f>Sheet1!C$7/C11</f>
+      <c r="F11" s="15">
+        <f>Sheet1!C$10/C11</f>
         <v>5.5034840000000003</v>
       </c>
-      <c r="G11" s="17">
-        <f>Sheet1!D$7/D11</f>
+      <c r="G11" s="15">
+        <f>Sheet1!D$10/D11</f>
         <v>32.064481481481479</v>
       </c>
-      <c r="H11" s="19">
-        <f>Sheet1!B$26/ICStoDCP!B11</f>
-        <v>0.46875</v>
-      </c>
-      <c r="I11" s="19">
-        <f>Sheet1!C$26/ICStoDCP!C11</f>
-        <v>1.6</v>
-      </c>
-      <c r="J11" s="19">
-        <f>Sheet1!D$26/ICStoDCP!D11</f>
-        <v>11.111111111111111</v>
-      </c>
-      <c r="K11" s="18">
-        <f>Sheet1!B$24/ICStoDCP!B11</f>
-        <v>0.15625</v>
-      </c>
-      <c r="L11" s="18">
-        <f>Sheet1!C$24/ICStoDCP!C11</f>
-        <v>1.6</v>
-      </c>
-      <c r="M11" s="18">
-        <f>Sheet1!D$24/ICStoDCP!D11</f>
-        <v>4.6296296296296298</v>
+      <c r="H11" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B11</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I11" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!C11</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J11" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D11</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K11" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B11</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L11" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!C11</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M11" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D11</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" s="7">
+      <c r="A12" s="6">
         <v>1035</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <v>640000</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <v>300000</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <v>27000</v>
       </c>
-      <c r="E12" s="17">
-        <f>Sheet1!B$7/B12</f>
+      <c r="E12" s="15">
+        <f>Sheet1!B$10/B12</f>
         <v>0.93553437500000003</v>
       </c>
-      <c r="F12" s="17">
-        <f>Sheet1!C$7/C12</f>
+      <c r="F12" s="15">
+        <f>Sheet1!C$10/C12</f>
         <v>4.5862366666666663</v>
       </c>
-      <c r="G12" s="17">
-        <f>Sheet1!D$7/D12</f>
+      <c r="G12" s="15">
+        <f>Sheet1!D$10/D12</f>
         <v>32.064481481481479</v>
       </c>
-      <c r="H12" s="19">
-        <f>Sheet1!B$26/ICStoDCP!B12</f>
-        <v>0.46875</v>
-      </c>
-      <c r="I12" s="19">
-        <f>Sheet1!C$26/ICStoDCP!C12</f>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="J12" s="19">
-        <f>Sheet1!D$26/ICStoDCP!D12</f>
-        <v>11.111111111111111</v>
-      </c>
-      <c r="K12" s="18">
-        <f>Sheet1!B$24/ICStoDCP!B12</f>
-        <v>0.15625</v>
-      </c>
-      <c r="L12" s="18">
-        <f>Sheet1!C$24/ICStoDCP!C12</f>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="M12" s="18">
-        <f>Sheet1!D$24/ICStoDCP!D12</f>
-        <v>4.6296296296296298</v>
+      <c r="H12" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B12</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I12" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!C12</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J12" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D12</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K12" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B12</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L12" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!C12</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M12" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D12</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" s="7">
+      <c r="A13" s="6">
         <v>1030</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>640000</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>350000</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <v>27000</v>
       </c>
-      <c r="E13" s="17">
-        <f>Sheet1!B$7/B13</f>
+      <c r="E13" s="15">
+        <f>Sheet1!B$10/B13</f>
         <v>0.93553437500000003</v>
       </c>
-      <c r="F13" s="17">
-        <f>Sheet1!C$7/C13</f>
+      <c r="F13" s="15">
+        <f>Sheet1!C$10/C13</f>
         <v>3.93106</v>
       </c>
-      <c r="G13" s="17">
-        <f>Sheet1!D$7/D13</f>
+      <c r="G13" s="15">
+        <f>Sheet1!D$10/D13</f>
         <v>32.064481481481479</v>
       </c>
-      <c r="H13" s="19">
-        <f>Sheet1!B$26/ICStoDCP!B13</f>
-        <v>0.46875</v>
-      </c>
-      <c r="I13" s="19">
-        <f>Sheet1!C$26/ICStoDCP!C13</f>
-        <v>1.1428571428571428</v>
-      </c>
-      <c r="J13" s="19">
-        <f>Sheet1!D$26/ICStoDCP!D13</f>
-        <v>11.111111111111111</v>
-      </c>
-      <c r="K13" s="18">
-        <f>Sheet1!B$24/ICStoDCP!B13</f>
-        <v>0.15625</v>
-      </c>
-      <c r="L13" s="18">
-        <f>Sheet1!C$24/ICStoDCP!C13</f>
-        <v>1.1428571428571428</v>
-      </c>
-      <c r="M13" s="18">
-        <f>Sheet1!D$24/ICStoDCP!D13</f>
-        <v>4.6296296296296298</v>
+      <c r="H13" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B13</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I13" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!C13</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J13" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D13</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K13" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B13</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L13" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!C13</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M13" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D13</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" s="7">
+      <c r="A14" s="6">
         <v>1025</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="6">
         <v>720000</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <v>350000</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="6">
         <v>30000</v>
       </c>
-      <c r="E14" s="17">
-        <f>Sheet1!B$7/B14</f>
+      <c r="E14" s="15">
+        <f>Sheet1!B$10/B14</f>
         <v>0.83158611111111114</v>
       </c>
-      <c r="F14" s="17">
-        <f>Sheet1!C$7/C14</f>
+      <c r="F14" s="15">
+        <f>Sheet1!C$10/C14</f>
         <v>3.93106</v>
       </c>
-      <c r="G14" s="17">
-        <f>Sheet1!D$7/D14</f>
+      <c r="G14" s="15">
+        <f>Sheet1!D$10/D14</f>
         <v>28.858033333333335</v>
       </c>
-      <c r="H14" s="19">
-        <f>Sheet1!B$26/ICStoDCP!B14</f>
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="I14" s="19">
-        <f>Sheet1!C$26/ICStoDCP!C14</f>
-        <v>1.1428571428571428</v>
-      </c>
-      <c r="J14" s="19">
-        <f>Sheet1!D$26/ICStoDCP!D14</f>
-        <v>10</v>
-      </c>
-      <c r="K14" s="18">
-        <f>Sheet1!B$24/ICStoDCP!B14</f>
-        <v>0.1388888888888889</v>
-      </c>
-      <c r="L14" s="18">
-        <f>Sheet1!C$24/ICStoDCP!C14</f>
-        <v>1.1428571428571428</v>
-      </c>
-      <c r="M14" s="18">
-        <f>Sheet1!D$24/ICStoDCP!D14</f>
-        <v>4.166666666666667</v>
+      <c r="H14" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B14</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I14" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!C14</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J14" s="17" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D14</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K14" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!B14</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L14" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!C14</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M14" s="16" t="e">
+        <f>Sheet1!#REF!/ICStoDCP!D14</f>
+        <v>#REF!</v>
       </c>
     </row>
   </sheetData>
@@ -1881,12 +2096,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5677A93C-B5FC-4BA5-BB13-1487C002EEE5}">
-  <dimension ref="A2:I5"/>
+  <dimension ref="A2:I7"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C5"/>
+    <sheetView topLeftCell="C1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2013,22 +2228,28 @@
         <v>0</v>
       </c>
     </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F7" s="11">
+        <f>SUM(F3:F5)</f>
+        <v>55434</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D265CD-11FF-4B0E-A32F-7305DFCA8DC1}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="A42" sqref="A42:D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2166,7 +2387,7 @@
         <f>19798+28566+799+400000+2094</f>
         <v>451257</v>
       </c>
-      <c r="F9" s="13"/>
+      <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
@@ -2226,7 +2447,7 @@
         <f>77162+29870+2722+400000+3050</f>
         <v>512804</v>
       </c>
-      <c r="E13" s="13"/>
+      <c r="E13" s="11"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14">

</xml_diff>

<commit_message>
Added ICS deposit to area plot
</commit_message>
<xml_diff>
--- a/LakeMeadStorageICS/IntentionallyCreatedSurplus-Summary.xlsx
+++ b/LakeMeadStorageICS/IntentionallyCreatedSurplus-Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadStorageICS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23FF1E6-7E50-4B4C-9D47-4C3F6BFEC3D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1329A473-69B9-47FD-8A1C-F5930698B24F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20520" yWindow="-2640" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-1800" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -668,7 +668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
@@ -1360,7 +1360,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F9C09D6-2BEE-4EAC-9C47-48919B4DAC3E}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B7" sqref="B7:F7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update LakeMeadStorageICS with 2023 ICS data. Code works
</commit_message>
<xml_diff>
--- a/LakeMeadStorageICS/IntentionallyCreatedSurplus-Summary.xlsx
+++ b/LakeMeadStorageICS/IntentionallyCreatedSurplus-Summary.xlsx
@@ -5,19 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadStorageICS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\ICS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1329A473-69B9-47FD-8A1C-F5930698B24F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACF12E2-AA49-4594-8D0D-8D62EF378416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="-1800" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Capacities" sheetId="5" r:id="rId2"/>
-    <sheet name="ICStoDCP" sheetId="3" r:id="rId3"/>
-    <sheet name="DCPLogs" sheetId="4" r:id="rId4"/>
-    <sheet name="By User" sheetId="2" r:id="rId5"/>
+    <sheet name="ReadMe" sheetId="6" r:id="rId1"/>
+    <sheet name="Balances" sheetId="1" r:id="rId2"/>
+    <sheet name="Deposits" sheetId="7" r:id="rId3"/>
+    <sheet name="Capacities" sheetId="5" r:id="rId4"/>
+    <sheet name="ICStoDCP" sheetId="3" r:id="rId5"/>
+    <sheet name="DCPLogs" sheetId="4" r:id="rId6"/>
+    <sheet name="By User" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,8 +41,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="78">
   <si>
     <t>Data Sources:</t>
   </si>
@@ -87,9 +111,6 @@
     <t>Balance - Dec 2015 (AF)</t>
   </si>
   <si>
-    <t>Intentionally Created Surplus (Lake Mead) - Summary Accounting</t>
-  </si>
-  <si>
     <t>Assessment of Losses</t>
   </si>
   <si>
@@ -186,24 +207,12 @@
     <t>NV</t>
   </si>
   <si>
-    <t>Percent of DCP obligation ICS max withdrawal can meet</t>
-  </si>
-  <si>
-    <t>Percent of DCP obliation max ICS deposit can fund</t>
-  </si>
-  <si>
-    <t>Annual Addition</t>
-  </si>
-  <si>
     <t>Balance - Dec 2020 (AF)</t>
   </si>
   <si>
     <t>Mexico</t>
   </si>
   <si>
-    <t>MX</t>
-  </si>
-  <si>
     <t>Required DCP Contribution</t>
   </si>
   <si>
@@ -235,6 +244,60 @@
   </si>
   <si>
     <t>Balance - Dec 2023 (AF)</t>
+  </si>
+  <si>
+    <t>Balance - Dec 2009 (AF)</t>
+  </si>
+  <si>
+    <t>Balance - Dec 2008 (AF)</t>
+  </si>
+  <si>
+    <t>Balance - Dec 2007 (AF)</t>
+  </si>
+  <si>
+    <t>Lake Mead Water Conservation Accounts (Intentionally Created Surplus) Data</t>
+  </si>
+  <si>
+    <t>Worksheet</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>1. Balances</t>
+  </si>
+  <si>
+    <t>Water Conservation account balances, credits, and debits, by year and entity.</t>
+  </si>
+  <si>
+    <t>Maximum credits, debits, and totals allowed per year</t>
+  </si>
+  <si>
+    <t>Explanation of how users met drought contingency plan (DPC) required conservation.</t>
+  </si>
+  <si>
+    <t>Number of years state can use ICS balance to meet drought contingency plan (DCP) required conservation</t>
+  </si>
+  <si>
+    <t>2. Deposits</t>
+  </si>
+  <si>
+    <t>Annual deposits and withdraws calculated as the year to year difference in balances.</t>
+  </si>
+  <si>
+    <t>3. Capacities</t>
+  </si>
+  <si>
+    <t>4. ICStoDPC</t>
+  </si>
+  <si>
+    <t>5. DCPLogs</t>
+  </si>
+  <si>
+    <t>6. ByUser</t>
+  </si>
+  <si>
+    <t>Account balance by state and contractor</t>
   </si>
 </sst>
 </file>
@@ -270,7 +333,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -286,6 +349,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCCCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -323,12 +392,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -361,11 +429,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -375,7 +438,11 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -385,10 +452,9 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -665,11 +731,110 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049640DB-DC1D-4720-8967-8C163BD4DD2C}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.453125" customWidth="1"/>
+    <col min="2" max="2" width="46.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -680,688 +845,1051 @@
     <col min="4" max="5" width="10.54296875" customWidth="1"/>
     <col min="6" max="6" width="11.7265625" customWidth="1"/>
     <col min="7" max="7" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.81640625" customWidth="1"/>
-    <col min="10" max="10" width="9.81640625" customWidth="1"/>
-    <col min="14" max="14" width="10.81640625" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="H5" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-    </row>
-    <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>41398</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <f>SUM(B2:E2)</f>
+        <v>41398</v>
+      </c>
+      <c r="G2" s="10">
+        <v>2007</v>
+      </c>
+      <c r="H2" s="11">
+        <f t="shared" ref="H2:H13" si="0">SUM(E2:F2)</f>
+        <v>41398</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="2">
+        <v>100000</v>
+      </c>
+      <c r="C3" s="2">
+        <f>27573+66000</f>
+        <v>93573</v>
+      </c>
+      <c r="D3" s="2">
+        <v>400000</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <f t="shared" ref="F3:F18" si="1">SUM(B3:D3)</f>
+        <v>593573</v>
+      </c>
+      <c r="G3" s="10">
+        <v>2008</v>
+      </c>
+      <c r="H3" s="11">
+        <f t="shared" si="0"/>
+        <v>593573</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="2">
+        <v>100000</v>
+      </c>
+      <c r="C4" s="2">
+        <f>79790+66000+11400</f>
+        <v>157190</v>
+      </c>
+      <c r="D4" s="2">
+        <v>400000</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" si="1"/>
+        <v>657190</v>
+      </c>
+      <c r="G4" s="10">
+        <v>2009</v>
+      </c>
+      <c r="H4" s="11">
+        <f t="shared" si="0"/>
+        <v>657190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="2">
+        <v>102094</v>
+      </c>
+      <c r="C5" s="2">
+        <v>261990</v>
+      </c>
+      <c r="D5" s="2">
+        <v>451257</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <f>SUM(B5:E5)</f>
+        <v>815341</v>
+      </c>
+      <c r="G5" s="10">
+        <v>2010</v>
+      </c>
+      <c r="H5" s="11">
+        <f t="shared" si="0"/>
+        <v>815341</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G6,'By User'!$C$2:$C$43,Balances!B$1)</f>
+        <v>103050</v>
+      </c>
+      <c r="C6" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G6,'By User'!$C$2:$C$43,Balances!C$1)</f>
+        <v>440678</v>
+      </c>
+      <c r="D6" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G6,'By User'!$C$2:$C$43,Balances!D$1)</f>
+        <v>482672</v>
+      </c>
+      <c r="E6" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G6,'By User'!$C$2:$C$43,Balances!E$1)</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="1"/>
+        <v>1026400</v>
+      </c>
+      <c r="G6" s="10">
+        <v>2011</v>
+      </c>
+      <c r="H6" s="11">
+        <f t="shared" si="0"/>
+        <v>1026400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G7,'By User'!$C$2:$C$43,Balances!B$1)</f>
+        <v>103050</v>
+      </c>
+      <c r="C7" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G7,'By User'!$C$2:$C$43,Balances!C$1)</f>
+        <v>579786</v>
+      </c>
+      <c r="D7" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G7,'By User'!$C$2:$C$43,Balances!D$1)</f>
+        <v>512804</v>
+      </c>
+      <c r="E7" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G7,'By User'!$C$2:$C$43,Balances!E$1)</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="1"/>
+        <v>1195640</v>
+      </c>
+      <c r="G7" s="10">
+        <v>2012</v>
+      </c>
+      <c r="H7" s="11">
+        <f t="shared" si="0"/>
+        <v>1195640</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G8,'By User'!$C$2:$C$43,Balances!B$1)</f>
+        <v>103050</v>
+      </c>
+      <c r="C8" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G8,'By User'!$C$2:$C$43,Balances!C$1)</f>
+        <v>474063</v>
+      </c>
+      <c r="D8" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G8,'By User'!$C$2:$C$43,Balances!D$1)</f>
+        <v>541051</v>
+      </c>
+      <c r="E8" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G8,'By User'!$C$2:$C$43,Balances!E$1)</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="1"/>
+        <v>1118164</v>
+      </c>
+      <c r="G8" s="10">
+        <v>2013</v>
+      </c>
+      <c r="H8" s="11">
+        <f t="shared" si="0"/>
+        <v>1118164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="K6" s="3" t="s">
+      <c r="B9" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G9,'By User'!$C$2:$C$43,Balances!B$1)</f>
+        <v>103050</v>
+      </c>
+      <c r="C9" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G9,'By User'!$C$2:$C$43,Balances!C$1)</f>
+        <v>169085</v>
+      </c>
+      <c r="D9" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G9,'By User'!$C$2:$C$43,Balances!D$1)</f>
+        <v>564765</v>
+      </c>
+      <c r="E9" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G9,'By User'!$C$2:$C$43,Balances!E$1)</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="1"/>
+        <v>836900</v>
+      </c>
+      <c r="G9" s="10">
+        <v>2014</v>
+      </c>
+      <c r="H9" s="11">
+        <f t="shared" si="0"/>
+        <v>836900</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G10,'By User'!$C$2:$C$43,Balances!B$1)</f>
+        <v>103050</v>
+      </c>
+      <c r="C10" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G10,'By User'!$C$2:$C$43,Balances!C$1)</f>
+        <v>97791</v>
+      </c>
+      <c r="D10" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G10,'By User'!$C$2:$C$43,Balances!D$1)</f>
+        <v>511023</v>
+      </c>
+      <c r="E10" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G10,'By User'!$C$2:$C$43,Balances!E$1)</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="1"/>
+        <v>711864</v>
+      </c>
+      <c r="G10" s="10">
+        <v>2015</v>
+      </c>
+      <c r="H10" s="11">
+        <f t="shared" si="0"/>
+        <v>711864</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G11,'By User'!$C$2:$C$43,Balances!B$1)</f>
+        <v>103050</v>
+      </c>
+      <c r="C11" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G11,'By User'!$C$2:$C$43,Balances!C$1)</f>
+        <v>115066</v>
+      </c>
+      <c r="D11" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G11,'By User'!$C$2:$C$43,Balances!D$1)</f>
+        <v>531562</v>
+      </c>
+      <c r="E11" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G11,'By User'!$C$2:$C$43,Balances!E$1)</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="1"/>
+        <v>749678</v>
+      </c>
+      <c r="G11" s="10">
+        <v>2016</v>
+      </c>
+      <c r="H11" s="11">
+        <f t="shared" si="0"/>
+        <v>749678</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G12,'By User'!$C$2:$C$43,Balances!B$1)</f>
+        <v>126800</v>
+      </c>
+      <c r="C12" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G12,'By User'!$C$2:$C$43,Balances!C$1)</f>
+        <v>552378</v>
+      </c>
+      <c r="D12" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G12,'By User'!$C$2:$C$43,Balances!D$1)</f>
+        <v>582313</v>
+      </c>
+      <c r="E12" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G12,'By User'!$C$2:$C$43,Balances!E$1)</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" si="1"/>
+        <v>1261491</v>
+      </c>
+      <c r="G12" s="10">
+        <v>2017</v>
+      </c>
+      <c r="H12" s="11">
+        <f t="shared" si="0"/>
+        <v>1261491</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G13,'By User'!$C$2:$C$43,Balances!B$1)</f>
+        <v>343052</v>
+      </c>
+      <c r="C13" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G13,'By User'!$C$2:$C$43,Balances!C$1)</f>
+        <v>698432</v>
+      </c>
+      <c r="D13" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G13,'By User'!$C$2:$C$43,Balances!D$1)</f>
+        <v>700448</v>
+      </c>
+      <c r="E13" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G13,'By User'!$C$2:$C$43,Balances!E$1)</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="1"/>
+        <v>1741932</v>
+      </c>
+      <c r="G13" s="9">
+        <v>2018</v>
+      </c>
+      <c r="H13" s="11">
+        <f t="shared" si="0"/>
+        <v>1741932</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G14,'By User'!$C$2:$C$43,Balances!B$1)</f>
+        <v>473504</v>
+      </c>
+      <c r="C14" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G14,'By User'!$C$2:$C$43,Balances!C$1)</f>
+        <v>1053210</v>
+      </c>
+      <c r="D14" s="2">
+        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Balances!$G14,'By User'!$C$2:$C$43,Balances!D$1)</f>
+        <v>785913</v>
+      </c>
+      <c r="E14" s="2">
+        <v>132975</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" si="1"/>
+        <v>2312627</v>
+      </c>
+      <c r="G14" s="12">
+        <v>2019</v>
+      </c>
+      <c r="H14" s="11">
+        <f>SUM(E14:F14)</f>
+        <v>2445602</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>47</v>
       </c>
-      <c r="L6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7" s="3">
+      <c r="B15" s="16">
+        <v>598742</v>
+      </c>
+      <c r="C15" s="16">
+        <v>1375871</v>
+      </c>
+      <c r="D15" s="16">
+        <v>865741</v>
+      </c>
+      <c r="E15" s="16">
+        <f>E14+41000</f>
+        <v>173975</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" si="1"/>
+        <v>2840354</v>
+      </c>
+      <c r="G15" s="17">
+        <v>2020</v>
+      </c>
+      <c r="H15" s="11">
+        <f>SUM(E15:F15)</f>
+        <v>3014329</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="16">
+        <v>684201</v>
+      </c>
+      <c r="C16" s="16">
+        <v>1357085</v>
+      </c>
+      <c r="D16" s="16">
+        <v>949658</v>
+      </c>
+      <c r="E16" s="16">
+        <f>E15+41000</f>
+        <v>214975</v>
+      </c>
+      <c r="F16" s="2">
+        <f t="shared" si="1"/>
+        <v>2990944</v>
+      </c>
+      <c r="G16" s="17">
+        <v>2021</v>
+      </c>
+      <c r="H16" s="11">
+        <f>SUM(E16:F16)</f>
+        <v>3205919</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="16">
+        <v>753423</v>
+      </c>
+      <c r="C17" s="16">
+        <v>1245693</v>
+      </c>
+      <c r="D17" s="16">
+        <v>1038765</v>
+      </c>
+      <c r="E17" s="16">
+        <f>30000+E16</f>
+        <v>244975</v>
+      </c>
+      <c r="F17" s="2">
+        <f t="shared" si="1"/>
+        <v>3037881</v>
+      </c>
+      <c r="G17" s="17">
+        <v>2022</v>
+      </c>
+      <c r="H17" s="11">
+        <f>SUM(E17:F17)</f>
+        <v>3282856</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="21">
         <v>710589</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C18" s="21">
         <v>1661832</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D18" s="21">
         <v>955543</v>
       </c>
-      <c r="E7" s="21">
-        <f>E8-34000</f>
+      <c r="E18" s="18">
+        <f>E17-34000</f>
         <v>210975</v>
       </c>
-      <c r="F7" s="2">
-        <f t="shared" ref="F7:F9" si="0">SUM(B7:D7)</f>
+      <c r="F18" s="2">
+        <f t="shared" si="1"/>
         <v>3327964</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G18" s="12">
         <v>2023</v>
       </c>
-      <c r="H7" s="11">
-        <f>F7-F8</f>
-        <v>290083</v>
-      </c>
-      <c r="I7" s="18">
-        <f t="shared" ref="I7" si="1">B7-B8</f>
-        <v>-42834</v>
-      </c>
-      <c r="J7" s="18">
-        <f t="shared" ref="J7" si="2">C7-C8</f>
-        <v>416139</v>
-      </c>
-      <c r="K7" s="18">
-        <f t="shared" ref="K7" si="3">D7-D8</f>
-        <v>-83222</v>
-      </c>
-      <c r="L7" s="18">
-        <f t="shared" ref="L7" si="4">E7-E8</f>
-        <v>-34000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" s="12">
-        <v>753423</v>
-      </c>
-      <c r="C8" s="12">
-        <v>1245693</v>
-      </c>
-      <c r="D8" s="12">
-        <v>1038765</v>
-      </c>
-      <c r="E8" s="19">
-        <f>30000+E9</f>
-        <v>244975</v>
-      </c>
-      <c r="F8" s="2">
-        <f t="shared" si="0"/>
-        <v>3037881</v>
-      </c>
-      <c r="G8" s="20">
-        <v>2022</v>
-      </c>
-      <c r="H8" s="11">
-        <f>F8-F9</f>
-        <v>46937</v>
-      </c>
-      <c r="I8" s="18">
-        <f t="shared" ref="I8:I9" si="5">B8-B9</f>
-        <v>69222</v>
-      </c>
-      <c r="J8" s="18">
-        <f t="shared" ref="J8:J9" si="6">C8-C9</f>
-        <v>-111392</v>
-      </c>
-      <c r="K8" s="18">
-        <f t="shared" ref="K8:K9" si="7">D8-D9</f>
-        <v>89107</v>
-      </c>
-      <c r="L8" s="18">
-        <f t="shared" ref="L8:L9" si="8">E8-E9</f>
-        <v>30000</v>
-      </c>
-      <c r="N8" s="11">
-        <f t="shared" ref="N8:N9" si="9">SUM(E8:F8)</f>
-        <v>3282856</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="12">
-        <v>684201</v>
-      </c>
-      <c r="C9" s="12">
-        <v>1357085</v>
-      </c>
-      <c r="D9" s="12">
-        <v>949658</v>
-      </c>
-      <c r="E9" s="19">
-        <f>41000+E10</f>
-        <v>214975</v>
-      </c>
-      <c r="F9" s="2">
-        <f t="shared" si="0"/>
-        <v>2990944</v>
-      </c>
-      <c r="G9" s="20">
-        <v>2021</v>
-      </c>
-      <c r="H9" s="11">
-        <f t="shared" ref="H9" si="10">F9-F10</f>
-        <v>150590</v>
-      </c>
-      <c r="I9" s="18">
-        <f t="shared" si="5"/>
-        <v>85459</v>
-      </c>
-      <c r="J9" s="18">
-        <f t="shared" si="6"/>
-        <v>-18786</v>
-      </c>
-      <c r="K9" s="18">
-        <f t="shared" si="7"/>
-        <v>83917</v>
-      </c>
-      <c r="L9" s="18">
-        <f t="shared" si="8"/>
-        <v>41000</v>
-      </c>
-      <c r="N9" s="11">
-        <f t="shared" si="9"/>
-        <v>3205919</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="19">
-        <v>598742</v>
-      </c>
-      <c r="C10" s="19">
-        <v>1375871</v>
-      </c>
-      <c r="D10" s="19">
-        <v>865741</v>
-      </c>
-      <c r="E10" s="19">
-        <f>41000+E11</f>
-        <v>173975</v>
-      </c>
-      <c r="F10" s="2">
-        <f>SUM(B10:D10)</f>
-        <v>2840354</v>
-      </c>
-      <c r="G10" s="20">
-        <v>2020</v>
-      </c>
-      <c r="H10" s="11">
-        <f>F10-F11</f>
-        <v>527727</v>
-      </c>
-      <c r="I10" s="18">
-        <f t="shared" ref="I10:L11" si="11">B10-B11</f>
-        <v>125238</v>
-      </c>
-      <c r="J10" s="18">
-        <f t="shared" si="11"/>
-        <v>322661</v>
-      </c>
-      <c r="K10" s="18">
-        <f t="shared" si="11"/>
-        <v>79828</v>
-      </c>
-      <c r="L10" s="18">
-        <f t="shared" si="11"/>
-        <v>41000</v>
-      </c>
-      <c r="N10" s="11">
-        <f>SUM(E10:F10)</f>
-        <v>3014329</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G11,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>473504</v>
-      </c>
-      <c r="C11" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G11,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>1053210</v>
-      </c>
-      <c r="D11" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G11,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>785913</v>
-      </c>
-      <c r="E11" s="2">
-        <v>132975</v>
-      </c>
-      <c r="F11" s="2">
-        <f>SUM(B11:D11)</f>
-        <v>2312627</v>
-      </c>
-      <c r="G11" s="12">
-        <v>2019</v>
-      </c>
-      <c r="H11" s="11">
-        <f>F11-F12</f>
-        <v>570695</v>
-      </c>
-      <c r="I11" s="18">
-        <f t="shared" si="11"/>
-        <v>130452</v>
-      </c>
-      <c r="J11" s="18">
-        <f t="shared" si="11"/>
-        <v>354778</v>
-      </c>
-      <c r="K11" s="18">
-        <f t="shared" si="11"/>
-        <v>85465</v>
-      </c>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18">
-        <f>H11-H10</f>
-        <v>42968</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G12,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>343052</v>
-      </c>
-      <c r="C12" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G12,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>698432</v>
-      </c>
-      <c r="D12" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G12,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>700448</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2">
-        <f>SUM(B12:D12)</f>
-        <v>1741932</v>
-      </c>
-      <c r="G12" s="9">
-        <v>2018</v>
-      </c>
-      <c r="H12" s="11">
-        <f>F12-F13</f>
-        <v>480441</v>
-      </c>
-      <c r="I12" s="18">
-        <f t="shared" ref="I12:I19" si="12">B12-B13</f>
-        <v>216252</v>
-      </c>
-      <c r="J12" s="18">
-        <f t="shared" ref="J12:J19" si="13">C12-C13</f>
-        <v>146054</v>
-      </c>
-      <c r="K12" s="18">
-        <f t="shared" ref="K12:K19" si="14">D12-D13</f>
-        <v>118135</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G13,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>126800</v>
-      </c>
-      <c r="C13" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G13,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>552378</v>
-      </c>
-      <c r="D13" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G13,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>582313</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2">
-        <f>SUM(B13:D13)</f>
-        <v>1261491</v>
-      </c>
-      <c r="G13" s="10">
-        <v>2017</v>
-      </c>
-      <c r="H13" s="11">
-        <f t="shared" ref="H13:H19" si="15">F13-F14</f>
-        <v>511813</v>
-      </c>
-      <c r="I13" s="18">
-        <f t="shared" si="12"/>
-        <v>23750</v>
-      </c>
-      <c r="J13" s="18">
-        <f t="shared" si="13"/>
-        <v>437312</v>
-      </c>
-      <c r="K13" s="18">
-        <f t="shared" si="14"/>
-        <v>50751</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G14,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>103050</v>
-      </c>
-      <c r="C14" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G14,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>115066</v>
-      </c>
-      <c r="D14" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G14,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>531562</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2">
-        <f t="shared" ref="F14:F20" si="16">SUM(B14:D14)</f>
-        <v>749678</v>
-      </c>
-      <c r="G14" s="10">
-        <v>2016</v>
-      </c>
-      <c r="H14" s="11">
-        <f t="shared" si="15"/>
-        <v>37814</v>
-      </c>
-      <c r="I14" s="18">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J14" s="18">
-        <f t="shared" si="13"/>
-        <v>17275</v>
-      </c>
-      <c r="K14" s="18">
-        <f t="shared" si="14"/>
-        <v>20539</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G15,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>103050</v>
-      </c>
-      <c r="C15" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G15,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>97791</v>
-      </c>
-      <c r="D15" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G15,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>511023</v>
-      </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2">
-        <f t="shared" si="16"/>
-        <v>711864</v>
-      </c>
-      <c r="G15" s="10">
-        <v>2015</v>
-      </c>
-      <c r="H15" s="11">
-        <f t="shared" si="15"/>
-        <v>-125036</v>
-      </c>
-      <c r="I15" s="18">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J15" s="18">
-        <f t="shared" si="13"/>
-        <v>-71294</v>
-      </c>
-      <c r="K15" s="18">
-        <f t="shared" si="14"/>
-        <v>-53742</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G16,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>103050</v>
-      </c>
-      <c r="C16" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G16,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>169085</v>
-      </c>
-      <c r="D16" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G16,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>564765</v>
-      </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2">
-        <f t="shared" si="16"/>
-        <v>836900</v>
-      </c>
-      <c r="G16" s="10">
-        <v>2014</v>
-      </c>
-      <c r="H16" s="11">
-        <f t="shared" si="15"/>
-        <v>-281264</v>
-      </c>
-      <c r="I16" s="18">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="18">
-        <f t="shared" si="13"/>
-        <v>-304978</v>
-      </c>
-      <c r="K16" s="18">
-        <f t="shared" si="14"/>
-        <v>23714</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G17,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>103050</v>
-      </c>
-      <c r="C17" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G17,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>474063</v>
-      </c>
-      <c r="D17" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G17,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>541051</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2">
-        <f t="shared" si="16"/>
-        <v>1118164</v>
-      </c>
-      <c r="G17" s="10">
-        <v>2013</v>
-      </c>
-      <c r="H17" s="11">
-        <f t="shared" si="15"/>
-        <v>-77476</v>
-      </c>
-      <c r="I17" s="18">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="18">
-        <f t="shared" si="13"/>
-        <v>-105723</v>
-      </c>
-      <c r="K17" s="18">
-        <f t="shared" si="14"/>
-        <v>28247</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G18,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>103050</v>
-      </c>
-      <c r="C18" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G18,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>579786</v>
-      </c>
-      <c r="D18" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G18,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>512804</v>
-      </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2">
-        <f t="shared" si="16"/>
-        <v>1195640</v>
-      </c>
-      <c r="G18" s="10">
-        <v>2012</v>
-      </c>
       <c r="H18" s="11">
-        <f t="shared" si="15"/>
-        <v>169240</v>
-      </c>
-      <c r="I18" s="18">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="18">
-        <f t="shared" si="13"/>
-        <v>139108</v>
-      </c>
-      <c r="K18" s="18">
-        <f t="shared" si="14"/>
-        <v>30132</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G19,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>103050</v>
-      </c>
-      <c r="C19" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G19,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>440678</v>
-      </c>
-      <c r="D19" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G19,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>482672</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2">
-        <f t="shared" si="16"/>
-        <v>1026400</v>
-      </c>
-      <c r="G19" s="10">
-        <v>2011</v>
-      </c>
-      <c r="H19" s="11">
-        <f t="shared" si="15"/>
-        <v>211059</v>
-      </c>
-      <c r="I19" s="18">
-        <f t="shared" si="12"/>
-        <v>956</v>
-      </c>
-      <c r="J19" s="18">
-        <f t="shared" si="13"/>
-        <v>178688</v>
-      </c>
-      <c r="K19" s="18">
-        <f t="shared" si="14"/>
-        <v>31415</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G20,'By User'!$C$2:$C$43,Sheet1!B$6)</f>
-        <v>102094</v>
-      </c>
-      <c r="C20" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G20,'By User'!$C$2:$C$43,Sheet1!C$6)</f>
-        <v>261990</v>
-      </c>
-      <c r="D20" s="2">
-        <f>SUMIFS('By User'!$D$2:$D$43,'By User'!$A$2:$A$43,Sheet1!$G20,'By User'!$C$2:$C$43,Sheet1!D$6)</f>
-        <v>451257</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2">
-        <f t="shared" si="16"/>
-        <v>815341</v>
-      </c>
-      <c r="G20" s="10">
-        <v>2010</v>
-      </c>
-      <c r="H20" s="11"/>
+        <f>SUM(E18:F18)</f>
+        <v>3538939</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="H5:K5"/>
-  </mergeCells>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H18">
+    <sortCondition ref="G2:G18"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83C452AE-E84E-4682-A6B7-6BBA39D2CE31}">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="12"/>
+    <col min="2" max="2" width="11.7265625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.1796875" style="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="str" cm="1">
+        <f t="array" ref="A1">Balances!G1:G1</f>
+        <v>Year</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="12">
+        <f>Balances!G2</f>
+        <v>2007</v>
+      </c>
+      <c r="B2" s="16">
+        <f>SUM(C2:F2)</f>
+        <v>41398</v>
+      </c>
+      <c r="C2" s="16">
+        <f>Balances!B2</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="16">
+        <f>Balances!C2</f>
+        <v>41398</v>
+      </c>
+      <c r="E2" s="16">
+        <f>Balances!D2</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="16">
+        <f>Balances!E3-Balances!E2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="12">
+        <f>Balances!G3</f>
+        <v>2008</v>
+      </c>
+      <c r="B3" s="16">
+        <f t="shared" ref="B3:B18" si="0">SUM(C3:F3)</f>
+        <v>552175</v>
+      </c>
+      <c r="C3" s="16">
+        <f>Balances!B3-Balances!B2</f>
+        <v>100000</v>
+      </c>
+      <c r="D3" s="16">
+        <f>Balances!C3-Balances!C2</f>
+        <v>52175</v>
+      </c>
+      <c r="E3" s="16">
+        <f>Balances!D3-Balances!D2</f>
+        <v>400000</v>
+      </c>
+      <c r="F3" s="16">
+        <f>Balances!E3-Balances!E2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="12">
+        <f>Balances!G4</f>
+        <v>2009</v>
+      </c>
+      <c r="B4" s="16">
+        <f t="shared" si="0"/>
+        <v>63617</v>
+      </c>
+      <c r="C4" s="16">
+        <f>Balances!B4-Balances!B3</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="16">
+        <f>Balances!C4-Balances!C3</f>
+        <v>63617</v>
+      </c>
+      <c r="E4" s="16">
+        <f>Balances!D4-Balances!D3</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="16">
+        <f>Balances!E4-Balances!E3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="12">
+        <f>Balances!G5</f>
+        <v>2010</v>
+      </c>
+      <c r="B5" s="16">
+        <f t="shared" si="0"/>
+        <v>158151</v>
+      </c>
+      <c r="C5" s="16">
+        <f>Balances!B5-Balances!B4</f>
+        <v>2094</v>
+      </c>
+      <c r="D5" s="16">
+        <f>Balances!C5-Balances!C4</f>
+        <v>104800</v>
+      </c>
+      <c r="E5" s="16">
+        <f>Balances!D5-Balances!D4</f>
+        <v>51257</v>
+      </c>
+      <c r="F5" s="16">
+        <f>Balances!E5-Balances!E4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="12">
+        <f>Balances!G6</f>
+        <v>2011</v>
+      </c>
+      <c r="B6" s="16">
+        <f t="shared" si="0"/>
+        <v>211059</v>
+      </c>
+      <c r="C6" s="16">
+        <f>Balances!B6-Balances!B5</f>
+        <v>956</v>
+      </c>
+      <c r="D6" s="16">
+        <f>Balances!C6-Balances!C5</f>
+        <v>178688</v>
+      </c>
+      <c r="E6" s="16">
+        <f>Balances!D6-Balances!D5</f>
+        <v>31415</v>
+      </c>
+      <c r="F6" s="16">
+        <f>Balances!E6-Balances!E5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="12">
+        <f>Balances!G7</f>
+        <v>2012</v>
+      </c>
+      <c r="B7" s="16">
+        <f t="shared" si="0"/>
+        <v>169240</v>
+      </c>
+      <c r="C7" s="16">
+        <f>Balances!B7-Balances!B6</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="16">
+        <f>Balances!C7-Balances!C6</f>
+        <v>139108</v>
+      </c>
+      <c r="E7" s="16">
+        <f>Balances!D7-Balances!D6</f>
+        <v>30132</v>
+      </c>
+      <c r="F7" s="16">
+        <f>Balances!E7-Balances!E6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="12">
+        <f>Balances!G8</f>
+        <v>2013</v>
+      </c>
+      <c r="B8" s="16">
+        <f t="shared" si="0"/>
+        <v>-77476</v>
+      </c>
+      <c r="C8" s="16">
+        <f>Balances!B8-Balances!B7</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="16">
+        <f>Balances!C8-Balances!C7</f>
+        <v>-105723</v>
+      </c>
+      <c r="E8" s="16">
+        <f>Balances!D8-Balances!D7</f>
+        <v>28247</v>
+      </c>
+      <c r="F8" s="16">
+        <f>Balances!E8-Balances!E7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="12">
+        <f>Balances!G9</f>
+        <v>2014</v>
+      </c>
+      <c r="B9" s="16">
+        <f t="shared" si="0"/>
+        <v>-281264</v>
+      </c>
+      <c r="C9" s="16">
+        <f>Balances!B9-Balances!B8</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="16">
+        <f>Balances!C9-Balances!C8</f>
+        <v>-304978</v>
+      </c>
+      <c r="E9" s="16">
+        <f>Balances!D9-Balances!D8</f>
+        <v>23714</v>
+      </c>
+      <c r="F9" s="16">
+        <f>Balances!E9-Balances!E8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="12">
+        <f>Balances!G10</f>
+        <v>2015</v>
+      </c>
+      <c r="B10" s="16">
+        <f t="shared" si="0"/>
+        <v>-125036</v>
+      </c>
+      <c r="C10" s="16">
+        <f>Balances!B10-Balances!B9</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="16">
+        <f>Balances!C10-Balances!C9</f>
+        <v>-71294</v>
+      </c>
+      <c r="E10" s="16">
+        <f>Balances!D10-Balances!D9</f>
+        <v>-53742</v>
+      </c>
+      <c r="F10" s="16">
+        <f>Balances!E10-Balances!E9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="12">
+        <f>Balances!G11</f>
+        <v>2016</v>
+      </c>
+      <c r="B11" s="16">
+        <f t="shared" si="0"/>
+        <v>37814</v>
+      </c>
+      <c r="C11" s="16">
+        <f>Balances!B11-Balances!B10</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="16">
+        <f>Balances!C11-Balances!C10</f>
+        <v>17275</v>
+      </c>
+      <c r="E11" s="16">
+        <f>Balances!D11-Balances!D10</f>
+        <v>20539</v>
+      </c>
+      <c r="F11" s="16">
+        <f>Balances!E11-Balances!E10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="12">
+        <f>Balances!G12</f>
+        <v>2017</v>
+      </c>
+      <c r="B12" s="16">
+        <f t="shared" si="0"/>
+        <v>511813</v>
+      </c>
+      <c r="C12" s="16">
+        <f>Balances!B12-Balances!B11</f>
+        <v>23750</v>
+      </c>
+      <c r="D12" s="16">
+        <f>Balances!C12-Balances!C11</f>
+        <v>437312</v>
+      </c>
+      <c r="E12" s="16">
+        <f>Balances!D12-Balances!D11</f>
+        <v>50751</v>
+      </c>
+      <c r="F12" s="16">
+        <f>Balances!E12-Balances!E11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="12">
+        <f>Balances!G13</f>
+        <v>2018</v>
+      </c>
+      <c r="B13" s="16">
+        <f t="shared" si="0"/>
+        <v>480441</v>
+      </c>
+      <c r="C13" s="16">
+        <f>Balances!B13-Balances!B12</f>
+        <v>216252</v>
+      </c>
+      <c r="D13" s="16">
+        <f>Balances!C13-Balances!C12</f>
+        <v>146054</v>
+      </c>
+      <c r="E13" s="16">
+        <f>Balances!D13-Balances!D12</f>
+        <v>118135</v>
+      </c>
+      <c r="F13" s="16">
+        <f>Balances!E13-Balances!E12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="12">
+        <f>Balances!G14</f>
+        <v>2019</v>
+      </c>
+      <c r="B14" s="16">
+        <f t="shared" si="0"/>
+        <v>703670</v>
+      </c>
+      <c r="C14" s="16">
+        <f>Balances!B14-Balances!B13</f>
+        <v>130452</v>
+      </c>
+      <c r="D14" s="16">
+        <f>Balances!C14-Balances!C13</f>
+        <v>354778</v>
+      </c>
+      <c r="E14" s="16">
+        <f>Balances!D14-Balances!D13</f>
+        <v>85465</v>
+      </c>
+      <c r="F14" s="16">
+        <f>Balances!E14-Balances!E13</f>
+        <v>132975</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="12">
+        <f>Balances!G15</f>
+        <v>2020</v>
+      </c>
+      <c r="B15" s="16">
+        <f t="shared" si="0"/>
+        <v>568727</v>
+      </c>
+      <c r="C15" s="16">
+        <f>Balances!B15-Balances!B14</f>
+        <v>125238</v>
+      </c>
+      <c r="D15" s="16">
+        <f>Balances!C15-Balances!C14</f>
+        <v>322661</v>
+      </c>
+      <c r="E15" s="16">
+        <f>Balances!D15-Balances!D14</f>
+        <v>79828</v>
+      </c>
+      <c r="F15" s="16">
+        <f>Balances!E15-Balances!E14</f>
+        <v>41000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="12">
+        <f>Balances!G16</f>
+        <v>2021</v>
+      </c>
+      <c r="B16" s="16">
+        <f t="shared" si="0"/>
+        <v>191590</v>
+      </c>
+      <c r="C16" s="16">
+        <f>Balances!B16-Balances!B15</f>
+        <v>85459</v>
+      </c>
+      <c r="D16" s="16">
+        <f>Balances!C16-Balances!C15</f>
+        <v>-18786</v>
+      </c>
+      <c r="E16" s="16">
+        <f>Balances!D16-Balances!D15</f>
+        <v>83917</v>
+      </c>
+      <c r="F16" s="16">
+        <f>Balances!E16-Balances!E15</f>
+        <v>41000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="12">
+        <f>Balances!G17</f>
+        <v>2022</v>
+      </c>
+      <c r="B17" s="16">
+        <f t="shared" si="0"/>
+        <v>76937</v>
+      </c>
+      <c r="C17" s="16">
+        <f>Balances!B17-Balances!B16</f>
+        <v>69222</v>
+      </c>
+      <c r="D17" s="16">
+        <f>Balances!C17-Balances!C16</f>
+        <v>-111392</v>
+      </c>
+      <c r="E17" s="16">
+        <f>Balances!D17-Balances!D16</f>
+        <v>89107</v>
+      </c>
+      <c r="F17" s="16">
+        <f>Balances!E17-Balances!E16</f>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="12">
+        <f>Balances!G18</f>
+        <v>2023</v>
+      </c>
+      <c r="B18" s="16">
+        <f t="shared" si="0"/>
+        <v>256083</v>
+      </c>
+      <c r="C18" s="16">
+        <f>Balances!B18-Balances!B17</f>
+        <v>-42834</v>
+      </c>
+      <c r="D18" s="16">
+        <f>Balances!C18-Balances!C17</f>
+        <v>416139</v>
+      </c>
+      <c r="E18" s="16">
+        <f>Balances!D18-Balances!D17</f>
+        <v>-83222</v>
+      </c>
+      <c r="F18" s="16">
+        <f>Balances!E18-Balances!E17</f>
+        <v>-34000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F9C09D6-2BEE-4EAC-9C47-48919B4DAC3E}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1385,7 +1913,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>6</v>
@@ -1450,7 +1978,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1467,7 +1995,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="8" t="str">
         <f>B1</f>
@@ -1511,7 +2039,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="6">
         <v>500000</v>
@@ -1551,18 +2079,18 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="A11" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1579,7 +2107,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -1599,7 +2127,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="4">
         <v>0.03</v>
@@ -1620,12 +2148,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F1C2B7-EA8A-46B6-A876-EE2A69C03180}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="H1" sqref="H1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1635,61 +2163,37 @@
     <col min="4" max="4" width="9.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="E1" s="24" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E1" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+    </row>
+    <row r="2" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="G2" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="14">
         <v>1218.5</v>
       </c>
@@ -1697,7 +2201,7 @@
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="14">
         <v>1190</v>
       </c>
@@ -1705,7 +2209,7 @@
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="14">
         <v>1150</v>
       </c>
@@ -1713,7 +2217,7 @@
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>1091</v>
       </c>
@@ -1721,7 +2225,7 @@
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>1090</v>
       </c>
@@ -1733,34 +2237,16 @@
         <v>8000</v>
       </c>
       <c r="E7" s="15">
-        <f>Sheet1!B$10/B7</f>
-        <v>3.1184479166666668</v>
+        <f>Balances!B$5/B7</f>
+        <v>0.53173958333333338</v>
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="15">
-        <f>Sheet1!D$10/D7</f>
-        <v>108.217625</v>
-      </c>
-      <c r="H7" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B7</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D7</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K7" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B7</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D7</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+        <f>Balances!D$5/D7</f>
+        <v>56.407125000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>1075</v>
       </c>
@@ -1772,34 +2258,16 @@
         <v>21000</v>
       </c>
       <c r="E8" s="15">
-        <f>Sheet1!B$10/B8</f>
-        <v>1.1694179687499999</v>
+        <f>Balances!B$5/B8</f>
+        <v>0.19940234374999999</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="15">
-        <f>Sheet1!D$10/D8</f>
-        <v>41.225761904761903</v>
-      </c>
-      <c r="H8" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B8</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D8</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K8" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B8</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D8</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+        <f>Balances!D$5/D8</f>
+        <v>21.488428571428571</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>1050</v>
       </c>
@@ -1811,34 +2279,16 @@
         <v>25000</v>
       </c>
       <c r="E9" s="15">
-        <f>Sheet1!B$10/B9</f>
-        <v>1.0113885135135134</v>
+        <f>Balances!B$5/B9</f>
+        <v>0.17245608108108107</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="15">
-        <f>Sheet1!D$10/D9</f>
-        <v>34.629640000000002</v>
-      </c>
-      <c r="H9" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B9</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D9</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K9" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B9</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D9</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+        <f>Balances!D$5/D9</f>
+        <v>18.050280000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>1045</v>
       </c>
@@ -1852,43 +2302,19 @@
         <v>27000</v>
       </c>
       <c r="E10" s="15">
-        <f>Sheet1!B$10/B10</f>
-        <v>0.93553437500000003</v>
+        <f>Balances!B$5/B10</f>
+        <v>0.15952187500000001</v>
       </c>
       <c r="F10" s="15">
-        <f>Sheet1!C$10/C10</f>
-        <v>6.8793550000000003</v>
+        <f>Balances!C$5/C10</f>
+        <v>1.3099499999999999</v>
       </c>
       <c r="G10" s="15">
-        <f>Sheet1!D$10/D10</f>
-        <v>32.064481481481479</v>
-      </c>
-      <c r="H10" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B10</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I10" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!C10</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J10" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D10</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K10" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B10</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L10" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!C10</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M10" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D10</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+        <f>Balances!D$5/D10</f>
+        <v>16.713222222222221</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <v>1040</v>
       </c>
@@ -1902,43 +2328,19 @@
         <v>27000</v>
       </c>
       <c r="E11" s="15">
-        <f>Sheet1!B$10/B11</f>
-        <v>0.93553437500000003</v>
+        <f>Balances!B$5/B11</f>
+        <v>0.15952187500000001</v>
       </c>
       <c r="F11" s="15">
-        <f>Sheet1!C$10/C11</f>
-        <v>5.5034840000000003</v>
+        <f>Balances!C$5/C11</f>
+        <v>1.04796</v>
       </c>
       <c r="G11" s="15">
-        <f>Sheet1!D$10/D11</f>
-        <v>32.064481481481479</v>
-      </c>
-      <c r="H11" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B11</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I11" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!C11</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J11" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D11</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K11" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B11</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L11" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!C11</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M11" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D11</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+        <f>Balances!D$5/D11</f>
+        <v>16.713222222222221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>1035</v>
       </c>
@@ -1952,43 +2354,19 @@
         <v>27000</v>
       </c>
       <c r="E12" s="15">
-        <f>Sheet1!B$10/B12</f>
-        <v>0.93553437500000003</v>
+        <f>Balances!B$5/B12</f>
+        <v>0.15952187500000001</v>
       </c>
       <c r="F12" s="15">
-        <f>Sheet1!C$10/C12</f>
-        <v>4.5862366666666663</v>
+        <f>Balances!C$5/C12</f>
+        <v>0.87329999999999997</v>
       </c>
       <c r="G12" s="15">
-        <f>Sheet1!D$10/D12</f>
-        <v>32.064481481481479</v>
-      </c>
-      <c r="H12" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B12</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I12" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!C12</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J12" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D12</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K12" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B12</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L12" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!C12</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M12" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D12</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+        <f>Balances!D$5/D12</f>
+        <v>16.713222222222221</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
         <v>1030</v>
       </c>
@@ -2002,43 +2380,19 @@
         <v>27000</v>
       </c>
       <c r="E13" s="15">
-        <f>Sheet1!B$10/B13</f>
-        <v>0.93553437500000003</v>
+        <f>Balances!B$5/B13</f>
+        <v>0.15952187500000001</v>
       </c>
       <c r="F13" s="15">
-        <f>Sheet1!C$10/C13</f>
-        <v>3.93106</v>
+        <f>Balances!C$5/C13</f>
+        <v>0.74854285714285718</v>
       </c>
       <c r="G13" s="15">
-        <f>Sheet1!D$10/D13</f>
-        <v>32.064481481481479</v>
-      </c>
-      <c r="H13" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B13</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I13" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!C13</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J13" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D13</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K13" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B13</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L13" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!C13</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M13" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D13</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+        <f>Balances!D$5/D13</f>
+        <v>16.713222222222221</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
         <v>1025</v>
       </c>
@@ -2052,40 +2406,16 @@
         <v>30000</v>
       </c>
       <c r="E14" s="15">
-        <f>Sheet1!B$10/B14</f>
-        <v>0.83158611111111114</v>
+        <f>Balances!B$5/B14</f>
+        <v>0.14179722222222221</v>
       </c>
       <c r="F14" s="15">
-        <f>Sheet1!C$10/C14</f>
-        <v>3.93106</v>
+        <f>Balances!C$5/C14</f>
+        <v>0.74854285714285718</v>
       </c>
       <c r="G14" s="15">
-        <f>Sheet1!D$10/D14</f>
-        <v>28.858033333333335</v>
-      </c>
-      <c r="H14" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B14</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I14" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!C14</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J14" s="17" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D14</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K14" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!B14</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L14" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!C14</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M14" s="16" t="e">
-        <f>Sheet1!#REF!/ICStoDCP!D14</f>
-        <v>#REF!</v>
+        <f>Balances!D$5/D14</f>
+        <v>15.0419</v>
       </c>
     </row>
   </sheetData>
@@ -2096,7 +2426,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5677A93C-B5FC-4BA5-BB13-1487C002EEE5}">
   <dimension ref="A2:I7"/>
   <sheetViews>
@@ -2115,31 +2445,31 @@
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" t="s">
         <v>54</v>
-      </c>
-      <c r="E2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H2" t="s">
-        <v>58</v>
-      </c>
-      <c r="I2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -2147,7 +2477,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C3">
         <v>2020</v>
@@ -2204,7 +2534,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5">
         <v>2020</v>
@@ -2239,11 +2569,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D265CD-11FF-4B0E-A32F-7305DFCA8DC1}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A42" sqref="A42:D42"/>
     </sheetView>
   </sheetViews>
@@ -2255,16 +2585,16 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>31</v>
-      </c>
-      <c r="D1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -2272,7 +2602,7 @@
         <v>2011</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -2289,7 +2619,7 @@
         <v>2011</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -2304,7 +2634,7 @@
         <v>2011</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -2319,7 +2649,7 @@
         <v>2011</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -2334,7 +2664,7 @@
         <v>2010</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
@@ -2349,7 +2679,7 @@
         <v>2010</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -2364,7 +2694,7 @@
         <v>2010</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -2378,7 +2708,7 @@
         <v>2010</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -2394,7 +2724,7 @@
         <v>2012</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
@@ -2409,7 +2739,7 @@
         <v>2012</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -2424,7 +2754,7 @@
         <v>2012</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -2438,7 +2768,7 @@
         <v>2012</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -2454,7 +2784,7 @@
         <v>2013</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
@@ -2469,7 +2799,7 @@
         <v>2013</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -2484,7 +2814,7 @@
         <v>2013</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -2498,7 +2828,7 @@
         <v>2013</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -2513,7 +2843,7 @@
         <v>2014</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
         <v>3</v>
@@ -2528,7 +2858,7 @@
         <v>2014</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -2543,7 +2873,7 @@
         <v>2014</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -2557,7 +2887,7 @@
         <v>2014</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
@@ -2571,7 +2901,7 @@
         <v>2015</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" t="s">
         <v>3</v>
@@ -2586,7 +2916,7 @@
         <v>2015</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
@@ -2601,7 +2931,7 @@
         <v>2015</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -2615,7 +2945,7 @@
         <v>2015</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
@@ -2629,7 +2959,7 @@
         <v>2016</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C26" t="s">
         <v>3</v>
@@ -2644,7 +2974,7 @@
         <v>2016</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -2659,7 +2989,7 @@
         <v>2016</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -2673,7 +3003,7 @@
         <v>2016</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" t="s">
         <v>5</v>
@@ -2687,7 +3017,7 @@
         <v>2017</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C30" t="s">
         <v>3</v>
@@ -2701,7 +3031,7 @@
         <v>2017</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -2715,7 +3045,7 @@
         <v>2017</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -2729,7 +3059,7 @@
         <v>2017</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33" t="s">
         <v>5</v>
@@ -2743,7 +3073,7 @@
         <v>2018</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34" t="s">
         <v>3</v>
@@ -2757,7 +3087,7 @@
         <v>2018</v>
       </c>
       <c r="B35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
@@ -2771,7 +3101,7 @@
         <v>2018</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
@@ -2785,7 +3115,7 @@
         <v>2018</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C37" t="s">
         <v>5</v>
@@ -2799,7 +3129,7 @@
         <v>2019</v>
       </c>
       <c r="B38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C38" t="s">
         <v>3</v>
@@ -2813,7 +3143,7 @@
         <v>2019</v>
       </c>
       <c r="B39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C39" t="s">
         <v>3</v>
@@ -2827,7 +3157,7 @@
         <v>2019</v>
       </c>
       <c r="B40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C40" t="s">
         <v>3</v>
@@ -2841,7 +3171,7 @@
         <v>2019</v>
       </c>
       <c r="B41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
@@ -2855,7 +3185,7 @@
         <v>2019</v>
       </c>
       <c r="B42" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C42" t="s">
         <v>4</v>
@@ -2869,7 +3199,7 @@
         <v>2019</v>
       </c>
       <c r="B43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C43" t="s">
         <v>5</v>

</xml_diff>